<commit_message>
update visual census coordinate attribute names
</commit_message>
<xml_diff>
--- a/assets/modules/visual-census/marinegeo_spreadsheet_visual_census.xlsx
+++ b/assets/modules/visual-census/marinegeo_spreadsheet_visual_census.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\spreadsheets_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D129D3-C882-4AAA-ADBF-18DFDB461113}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0E9E23-2CBC-4286-975C-1F1D714EBE81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31575" yWindow="2685" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -360,12 +360,6 @@
     <t>buddy</t>
   </si>
   <si>
-    <t>transect_decimal_latitude</t>
-  </si>
-  <si>
-    <t>transect_decimal_longitude</t>
-  </si>
-  <si>
     <t>depth_m</t>
   </si>
   <si>
@@ -475,6 +469,12 @@
   </si>
   <si>
     <t>v0.5.0</t>
+  </si>
+  <si>
+    <t>transect_begin_decimal_latitude</t>
+  </si>
+  <si>
+    <t>transect_begin_decimal_longitude</t>
   </si>
 </sst>
 </file>
@@ -1486,7 +1486,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="161.1" customHeight="1">
       <c r="B1" s="62" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1511,19 +1511,19 @@
     </row>
     <row r="5" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B5" s="9"/>
     </row>
     <row r="6" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B7" s="9"/>
     </row>
@@ -1544,7 +1544,7 @@
         <v>86</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1552,7 +1552,7 @@
         <v>87</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1620,7 +1620,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1628,7 +1628,7 @@
     <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" style="1" customWidth="1"/>
     <col min="3" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
     <col min="8" max="9" width="19.140625" style="1" customWidth="1"/>
@@ -1642,7 +1642,7 @@
         <v>100</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C1" s="38" t="s">
         <v>99</v>
@@ -1651,13 +1651,13 @@
         <v>101</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H1" s="39" t="s">
         <v>102</v>
@@ -1669,16 +1669,16 @@
         <v>82</v>
       </c>
       <c r="K1" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="M1" s="39" t="s">
-        <v>108</v>
-      </c>
       <c r="N1" s="39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -4484,7 +4484,7 @@
         <v>100</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C1" s="38" t="s">
         <v>99</v>
@@ -4493,16 +4493,16 @@
         <v>101</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F1" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="43" t="s">
-        <v>111</v>
-      </c>
       <c r="H1" s="44" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I1" s="45">
         <v>2.5</v>
@@ -4589,7 +4589,7 @@
         <v>400</v>
       </c>
       <c r="AK1" s="48" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AL1" s="41"/>
       <c r="AM1" s="41"/>
@@ -6778,13 +6778,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="47" customFormat="1" ht="24" customHeight="1">
       <c r="A1" s="49" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B1" s="50" t="s">
         <v>97</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
@@ -8099,8 +8099,8 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="50.1" customHeight="1"/>
@@ -8330,7 +8330,7 @@
         <v>94</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>28</v>
@@ -8380,7 +8380,7 @@
         <v>94</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>30</v>
@@ -8398,7 +8398,7 @@
         <v>94</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>31</v>
@@ -8416,16 +8416,16 @@
         <v>94</v>
       </c>
       <c r="B19" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>128</v>
-      </c>
       <c r="E19" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F19" s="6"/>
     </row>
@@ -8469,7 +8469,7 @@
         <v>82</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
@@ -8482,7 +8482,7 @@
         <v>94</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>69</v>
@@ -8500,7 +8500,7 @@
         <v>94</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>68</v>
@@ -8520,7 +8520,7 @@
         <v>94</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>66</v>
@@ -8540,10 +8540,10 @@
         <v>94</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>17</v>
@@ -8568,7 +8568,7 @@
         <v>95</v>
       </c>
       <c r="B28" s="55" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>28</v>
@@ -8623,7 +8623,7 @@
         <v>101</v>
       </c>
       <c r="C31" s="57" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>29</v>
@@ -8636,10 +8636,10 @@
         <v>95</v>
       </c>
       <c r="B32" s="56" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>29</v>
@@ -8652,7 +8652,7 @@
         <v>95</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C33" s="24" t="s">
         <v>74</v>
@@ -8672,7 +8672,7 @@
         <v>95</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C34" s="25" t="s">
         <v>76</v>
@@ -8688,7 +8688,7 @@
         <v>95</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C35" s="25" t="s">
         <v>75</v>
@@ -9268,10 +9268,10 @@
         <v>95</v>
       </c>
       <c r="B64" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="25" t="s">
         <v>118</v>
-      </c>
-      <c r="C64" s="25" t="s">
-        <v>120</v>
       </c>
       <c r="D64" s="24" t="s">
         <v>17</v>
@@ -9296,10 +9296,10 @@
         <v>96</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>17</v>
@@ -9315,7 +9315,7 @@
         <v>97</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>17</v>
@@ -9328,10 +9328,10 @@
         <v>96</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>17</v>

</xml_diff>